<commit_message>
Nova tela de pesquisa
</commit_message>
<xml_diff>
--- a/GynLog/Veiculo.xlsx
+++ b/GynLog/Veiculo.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2006" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2010" uniqueCount="548">
   <si>
     <t>ID Veículo</t>
   </si>
@@ -41,18 +41,21 @@
     <t>Constellation</t>
   </si>
   <si>
+    <t>Disponível</t>
+  </si>
+  <si>
+    <t>IZG4199</t>
+  </si>
+  <si>
+    <t>Volvo</t>
+  </si>
+  <si>
+    <t>FMX</t>
+  </si>
+  <si>
     <t>Indisponível</t>
   </si>
   <si>
-    <t>IZG4199</t>
-  </si>
-  <si>
-    <t>Volvo</t>
-  </si>
-  <si>
-    <t>FMX</t>
-  </si>
-  <si>
     <t>UEG0B88</t>
   </si>
   <si>
@@ -119,9 +122,6 @@
     <t>Toro</t>
   </si>
   <si>
-    <t>Disponível</t>
-  </si>
-  <si>
     <t>TBI0J79</t>
   </si>
   <si>
@@ -1650,6 +1650,12 @@
   </si>
   <si>
     <t>KBM8T69</t>
+  </si>
+  <si>
+    <t>ABC1234</t>
+  </si>
+  <si>
+    <t>Amarok</t>
   </si>
 </sst>
 </file>
@@ -1694,7 +1700,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F501"/>
+  <dimension ref="A1:F502"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1765,7 +1771,7 @@
         <v>1996.0</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -1773,7 +1779,7 @@
         <v>100002.0</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>11</v>
@@ -1785,7 +1791,7 @@
         <v>2019.0</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
@@ -1793,13 +1799,13 @@
         <v>100003.0</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" t="n" s="0">
         <v>1993.0</v>
@@ -1813,19 +1819,19 @@
         <v>100004.0</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" t="n" s="0">
         <v>2013.0</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
@@ -1833,7 +1839,7 @@
         <v>100005.0</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>11</v>
@@ -1853,13 +1859,13 @@
         <v>100006.0</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" t="n" s="0">
         <v>2021.0</v>
@@ -1873,13 +1879,13 @@
         <v>100007.0</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9" t="n" s="0">
         <v>2007.0</v>
@@ -1893,19 +1899,19 @@
         <v>100008.0</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E10" t="n" s="0">
         <v>1997.0</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11">
@@ -1913,19 +1919,19 @@
         <v>100009.0</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s" s="0">
         <v>11</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E11" t="n" s="0">
         <v>1987.0</v>
       </c>
       <c r="F11" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12">
@@ -1933,19 +1939,19 @@
         <v>100010.0</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E12" t="n" s="0">
         <v>2013.0</v>
       </c>
       <c r="F12" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
@@ -1953,19 +1959,19 @@
         <v>100011.0</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E13" t="n" s="0">
         <v>1986.0</v>
       </c>
       <c r="F13" t="s" s="0">
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14">
@@ -1976,7 +1982,7 @@
         <v>36</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s" s="0">
         <v>37</v>
@@ -1996,7 +2002,7 @@
         <v>38</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s" s="0">
         <v>39</v>
@@ -2025,7 +2031,7 @@
         <v>2019.0</v>
       </c>
       <c r="F16" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17">
@@ -2076,16 +2082,16 @@
         <v>48</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E19" t="n" s="0">
         <v>2005.0</v>
       </c>
       <c r="F19" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20">
@@ -2145,7 +2151,7 @@
         <v>2008.0</v>
       </c>
       <c r="F22" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23">
@@ -2165,7 +2171,7 @@
         <v>2008.0</v>
       </c>
       <c r="F23" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24">
@@ -2176,7 +2182,7 @@
         <v>56</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s" s="0">
         <v>39</v>
@@ -2196,7 +2202,7 @@
         <v>57</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D25" t="s" s="0">
         <v>58</v>
@@ -2205,7 +2211,7 @@
         <v>1994.0</v>
       </c>
       <c r="F25" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26">
@@ -2236,7 +2242,7 @@
         <v>61</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D27" t="s" s="0">
         <v>58</v>
@@ -2256,7 +2262,7 @@
         <v>62</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D28" t="s" s="0">
         <v>58</v>
@@ -2265,7 +2271,7 @@
         <v>1986.0</v>
       </c>
       <c r="F28" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29">
@@ -2285,7 +2291,7 @@
         <v>2025.0</v>
       </c>
       <c r="F29" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30">
@@ -2296,10 +2302,10 @@
         <v>64</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E30" t="n" s="0">
         <v>2025.0</v>
@@ -2325,7 +2331,7 @@
         <v>2001.0</v>
       </c>
       <c r="F31" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32">
@@ -2396,7 +2402,7 @@
         <v>70</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D35" t="s" s="0">
         <v>71</v>
@@ -2416,7 +2422,7 @@
         <v>72</v>
       </c>
       <c r="C36" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D36" t="s" s="0">
         <v>71</v>
@@ -2425,7 +2431,7 @@
         <v>1999.0</v>
       </c>
       <c r="F36" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37">
@@ -2476,7 +2482,7 @@
         <v>76</v>
       </c>
       <c r="C39" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D39" t="s" s="0">
         <v>77</v>
@@ -2485,7 +2491,7 @@
         <v>2000.0</v>
       </c>
       <c r="F39" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40">
@@ -2516,10 +2522,10 @@
         <v>80</v>
       </c>
       <c r="C41" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D41" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E41" t="n" s="0">
         <v>2020.0</v>
@@ -2536,7 +2542,7 @@
         <v>81</v>
       </c>
       <c r="C42" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D42" t="s" s="0">
         <v>77</v>
@@ -2556,7 +2562,7 @@
         <v>82</v>
       </c>
       <c r="C43" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D43" t="s" s="0">
         <v>37</v>
@@ -2596,7 +2602,7 @@
         <v>84</v>
       </c>
       <c r="C45" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D45" t="s" s="0">
         <v>39</v>
@@ -2605,7 +2611,7 @@
         <v>2006.0</v>
       </c>
       <c r="F45" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46">
@@ -2625,7 +2631,7 @@
         <v>2013.0</v>
       </c>
       <c r="F46" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47">
@@ -2656,7 +2662,7 @@
         <v>87</v>
       </c>
       <c r="C48" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D48" t="s" s="0">
         <v>88</v>
@@ -2685,7 +2691,7 @@
         <v>2006.0</v>
       </c>
       <c r="F49" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50">
@@ -2696,7 +2702,7 @@
         <v>90</v>
       </c>
       <c r="C50" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D50" t="s" s="0">
         <v>77</v>
@@ -2716,7 +2722,7 @@
         <v>91</v>
       </c>
       <c r="C51" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D51" t="s" s="0">
         <v>37</v>
@@ -2736,10 +2742,10 @@
         <v>92</v>
       </c>
       <c r="C52" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D52" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E52" t="n" s="0">
         <v>2019.0</v>
@@ -2776,7 +2782,7 @@
         <v>94</v>
       </c>
       <c r="C54" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D54" t="s" s="0">
         <v>71</v>
@@ -2785,7 +2791,7 @@
         <v>2024.0</v>
       </c>
       <c r="F54" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55">
@@ -2796,7 +2802,7 @@
         <v>95</v>
       </c>
       <c r="C55" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D55" t="s" s="0">
         <v>77</v>
@@ -2805,7 +2811,7 @@
         <v>2013.0</v>
       </c>
       <c r="F55" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56">
@@ -2825,7 +2831,7 @@
         <v>2012.0</v>
       </c>
       <c r="F56" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57">
@@ -2876,10 +2882,10 @@
         <v>99</v>
       </c>
       <c r="C59" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D59" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E59" t="n" s="0">
         <v>2009.0</v>
@@ -2899,13 +2905,13 @@
         <v>11</v>
       </c>
       <c r="D60" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E60" t="n" s="0">
         <v>2005.0</v>
       </c>
       <c r="F60" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61">
@@ -2916,7 +2922,7 @@
         <v>101</v>
       </c>
       <c r="C61" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D61" t="s" s="0">
         <v>39</v>
@@ -2925,7 +2931,7 @@
         <v>1986.0</v>
       </c>
       <c r="F61" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62">
@@ -2945,7 +2951,7 @@
         <v>2024.0</v>
       </c>
       <c r="F62" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63">
@@ -2965,7 +2971,7 @@
         <v>2020.0</v>
       </c>
       <c r="F63" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="64">
@@ -2996,10 +3002,10 @@
         <v>105</v>
       </c>
       <c r="C65" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D65" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E65" t="n" s="0">
         <v>2001.0</v>
@@ -3016,7 +3022,7 @@
         <v>106</v>
       </c>
       <c r="C66" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D66" t="s" s="0">
         <v>107</v>
@@ -3045,7 +3051,7 @@
         <v>2022.0</v>
       </c>
       <c r="F67" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68">
@@ -3065,7 +3071,7 @@
         <v>2006.0</v>
       </c>
       <c r="F68" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="69">
@@ -3076,7 +3082,7 @@
         <v>111</v>
       </c>
       <c r="C69" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D69" t="s" s="0">
         <v>37</v>
@@ -3085,7 +3091,7 @@
         <v>2019.0</v>
       </c>
       <c r="F69" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70">
@@ -3105,7 +3111,7 @@
         <v>2020.0</v>
       </c>
       <c r="F70" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="71">
@@ -3116,7 +3122,7 @@
         <v>113</v>
       </c>
       <c r="C71" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D71" t="s" s="0">
         <v>58</v>
@@ -3136,16 +3142,16 @@
         <v>114</v>
       </c>
       <c r="C72" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D72" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E72" t="n" s="0">
         <v>2021.0</v>
       </c>
       <c r="F72" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="73">
@@ -3156,7 +3162,7 @@
         <v>115</v>
       </c>
       <c r="C73" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D73" t="s" s="0">
         <v>37</v>
@@ -3165,7 +3171,7 @@
         <v>1991.0</v>
       </c>
       <c r="F73" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="74">
@@ -3176,10 +3182,10 @@
         <v>116</v>
       </c>
       <c r="C74" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D74" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E74" t="n" s="0">
         <v>1987.0</v>
@@ -3196,7 +3202,7 @@
         <v>117</v>
       </c>
       <c r="C75" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D75" t="s" s="0">
         <v>37</v>
@@ -3216,7 +3222,7 @@
         <v>118</v>
       </c>
       <c r="C76" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D76" t="s" s="0">
         <v>71</v>
@@ -3225,7 +3231,7 @@
         <v>1992.0</v>
       </c>
       <c r="F76" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77">
@@ -3245,7 +3251,7 @@
         <v>2001.0</v>
       </c>
       <c r="F77" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78">
@@ -3256,16 +3262,16 @@
         <v>120</v>
       </c>
       <c r="C78" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D78" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E78" t="n" s="0">
         <v>2012.0</v>
       </c>
       <c r="F78" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="79">
@@ -3276,10 +3282,10 @@
         <v>121</v>
       </c>
       <c r="C79" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D79" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E79" t="n" s="0">
         <v>1997.0</v>
@@ -3356,16 +3362,16 @@
         <v>125</v>
       </c>
       <c r="C83" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D83" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E83" t="n" s="0">
         <v>1993.0</v>
       </c>
       <c r="F83" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84">
@@ -3376,16 +3382,16 @@
         <v>126</v>
       </c>
       <c r="C84" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D84" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E84" t="n" s="0">
         <v>2006.0</v>
       </c>
       <c r="F84" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="85">
@@ -3416,7 +3422,7 @@
         <v>128</v>
       </c>
       <c r="C86" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D86" t="s" s="0">
         <v>129</v>
@@ -3425,7 +3431,7 @@
         <v>1997.0</v>
       </c>
       <c r="F86" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87">
@@ -3436,16 +3442,16 @@
         <v>130</v>
       </c>
       <c r="C87" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D87" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E87" t="n" s="0">
         <v>1989.0</v>
       </c>
       <c r="F87" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="88">
@@ -3479,13 +3485,13 @@
         <v>11</v>
       </c>
       <c r="D89" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E89" t="n" s="0">
         <v>2003.0</v>
       </c>
       <c r="F89" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="90">
@@ -3505,7 +3511,7 @@
         <v>2005.0</v>
       </c>
       <c r="F90" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="91">
@@ -3536,16 +3542,16 @@
         <v>135</v>
       </c>
       <c r="C92" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D92" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E92" t="n" s="0">
         <v>1999.0</v>
       </c>
       <c r="F92" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="93">
@@ -3565,7 +3571,7 @@
         <v>1997.0</v>
       </c>
       <c r="F93" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="94">
@@ -3596,10 +3602,10 @@
         <v>138</v>
       </c>
       <c r="C95" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D95" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E95" t="n" s="0">
         <v>1997.0</v>
@@ -3645,7 +3651,7 @@
         <v>1990.0</v>
       </c>
       <c r="F97" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="98">
@@ -3665,7 +3671,7 @@
         <v>2020.0</v>
       </c>
       <c r="F98" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="99">
@@ -3676,7 +3682,7 @@
         <v>142</v>
       </c>
       <c r="C99" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D99" t="s" s="0">
         <v>88</v>
@@ -3699,13 +3705,13 @@
         <v>11</v>
       </c>
       <c r="D100" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E100" t="n" s="0">
         <v>2004.0</v>
       </c>
       <c r="F100" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="101">
@@ -3716,10 +3722,10 @@
         <v>144</v>
       </c>
       <c r="C101" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D101" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E101" t="n" s="0">
         <v>1996.0</v>
@@ -3745,7 +3751,7 @@
         <v>2025.0</v>
       </c>
       <c r="F102" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="103">
@@ -3765,7 +3771,7 @@
         <v>2021.0</v>
       </c>
       <c r="F103" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="104">
@@ -3785,7 +3791,7 @@
         <v>2019.0</v>
       </c>
       <c r="F104" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="105">
@@ -3805,7 +3811,7 @@
         <v>1985.0</v>
       </c>
       <c r="F105" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="106">
@@ -3825,7 +3831,7 @@
         <v>2002.0</v>
       </c>
       <c r="F106" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="107">
@@ -3856,7 +3862,7 @@
         <v>151</v>
       </c>
       <c r="C108" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D108" t="s" s="0">
         <v>37</v>
@@ -3876,16 +3882,16 @@
         <v>152</v>
       </c>
       <c r="C109" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D109" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E109" t="n" s="0">
         <v>2018.0</v>
       </c>
       <c r="F109" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="110">
@@ -3905,7 +3911,7 @@
         <v>2012.0</v>
       </c>
       <c r="F110" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="111">
@@ -3916,7 +3922,7 @@
         <v>154</v>
       </c>
       <c r="C111" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D111" t="s" s="0">
         <v>58</v>
@@ -3925,7 +3931,7 @@
         <v>2023.0</v>
       </c>
       <c r="F111" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="112">
@@ -3956,7 +3962,7 @@
         <v>156</v>
       </c>
       <c r="C113" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D113" t="s" s="0">
         <v>37</v>
@@ -3965,7 +3971,7 @@
         <v>1985.0</v>
       </c>
       <c r="F113" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="114">
@@ -3979,7 +3985,7 @@
         <v>11</v>
       </c>
       <c r="D114" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E114" t="n" s="0">
         <v>1986.0</v>
@@ -3996,7 +4002,7 @@
         <v>158</v>
       </c>
       <c r="C115" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D115" t="s" s="0">
         <v>107</v>
@@ -4005,7 +4011,7 @@
         <v>1998.0</v>
       </c>
       <c r="F115" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="116">
@@ -4036,16 +4042,16 @@
         <v>160</v>
       </c>
       <c r="C117" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D117" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E117" t="n" s="0">
         <v>1993.0</v>
       </c>
       <c r="F117" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="118">
@@ -4076,10 +4082,10 @@
         <v>162</v>
       </c>
       <c r="C119" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D119" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E119" t="n" s="0">
         <v>2009.0</v>
@@ -4096,7 +4102,7 @@
         <v>163</v>
       </c>
       <c r="C120" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D120" t="s" s="0">
         <v>129</v>
@@ -4105,7 +4111,7 @@
         <v>1989.0</v>
       </c>
       <c r="F120" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="121">
@@ -4116,7 +4122,7 @@
         <v>164</v>
       </c>
       <c r="C121" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D121" t="s" s="0">
         <v>129</v>
@@ -4125,7 +4131,7 @@
         <v>2022.0</v>
       </c>
       <c r="F121" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="122">
@@ -4156,16 +4162,16 @@
         <v>166</v>
       </c>
       <c r="C123" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D123" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E123" t="n" s="0">
         <v>2010.0</v>
       </c>
       <c r="F123" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="124">
@@ -4179,7 +4185,7 @@
         <v>11</v>
       </c>
       <c r="D124" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E124" t="n" s="0">
         <v>2006.0</v>
@@ -4196,7 +4202,7 @@
         <v>168</v>
       </c>
       <c r="C125" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D125" t="s" s="0">
         <v>88</v>
@@ -4225,7 +4231,7 @@
         <v>2000.0</v>
       </c>
       <c r="F126" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="127">
@@ -4256,7 +4262,7 @@
         <v>171</v>
       </c>
       <c r="C128" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D128" t="s" s="0">
         <v>88</v>
@@ -4265,7 +4271,7 @@
         <v>2002.0</v>
       </c>
       <c r="F128" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="129">
@@ -4285,7 +4291,7 @@
         <v>2007.0</v>
       </c>
       <c r="F129" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="130">
@@ -4296,7 +4302,7 @@
         <v>173</v>
       </c>
       <c r="C130" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D130" t="s" s="0">
         <v>129</v>
@@ -4319,7 +4325,7 @@
         <v>11</v>
       </c>
       <c r="D131" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E131" t="n" s="0">
         <v>2006.0</v>
@@ -4336,7 +4342,7 @@
         <v>175</v>
       </c>
       <c r="C132" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D132" t="s" s="0">
         <v>88</v>
@@ -4365,7 +4371,7 @@
         <v>2007.0</v>
       </c>
       <c r="F133" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="134">
@@ -4385,7 +4391,7 @@
         <v>1999.0</v>
       </c>
       <c r="F134" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="135">
@@ -4425,7 +4431,7 @@
         <v>1993.0</v>
       </c>
       <c r="F136" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="137">
@@ -4445,7 +4451,7 @@
         <v>2019.0</v>
       </c>
       <c r="F137" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="138">
@@ -4456,16 +4462,16 @@
         <v>181</v>
       </c>
       <c r="C138" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D138" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E138" t="n" s="0">
         <v>2020.0</v>
       </c>
       <c r="F138" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="139">
@@ -4516,7 +4522,7 @@
         <v>184</v>
       </c>
       <c r="C141" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D141" t="s" s="0">
         <v>129</v>
@@ -4536,7 +4542,7 @@
         <v>185</v>
       </c>
       <c r="C142" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D142" t="s" s="0">
         <v>129</v>
@@ -4545,7 +4551,7 @@
         <v>1985.0</v>
       </c>
       <c r="F142" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="143">
@@ -4565,7 +4571,7 @@
         <v>2026.0</v>
       </c>
       <c r="F143" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="144">
@@ -4585,7 +4591,7 @@
         <v>2005.0</v>
       </c>
       <c r="F144" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="145">
@@ -4599,7 +4605,7 @@
         <v>11</v>
       </c>
       <c r="D145" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E145" t="n" s="0">
         <v>2012.0</v>
@@ -4616,7 +4622,7 @@
         <v>189</v>
       </c>
       <c r="C146" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D146" t="s" s="0">
         <v>58</v>
@@ -4625,7 +4631,7 @@
         <v>2002.0</v>
       </c>
       <c r="F146" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="147">
@@ -4645,7 +4651,7 @@
         <v>2001.0</v>
       </c>
       <c r="F147" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="148">
@@ -4656,7 +4662,7 @@
         <v>191</v>
       </c>
       <c r="C148" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D148" t="s" s="0">
         <v>107</v>
@@ -4676,10 +4682,10 @@
         <v>192</v>
       </c>
       <c r="C149" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D149" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E149" t="n" s="0">
         <v>1990.0</v>
@@ -4716,10 +4722,10 @@
         <v>194</v>
       </c>
       <c r="C151" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D151" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E151" t="n" s="0">
         <v>2012.0</v>
@@ -4736,7 +4742,7 @@
         <v>195</v>
       </c>
       <c r="C152" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D152" t="s" s="0">
         <v>88</v>
@@ -4745,7 +4751,7 @@
         <v>2004.0</v>
       </c>
       <c r="F152" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="153">
@@ -4765,7 +4771,7 @@
         <v>1996.0</v>
       </c>
       <c r="F153" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="154">
@@ -4779,7 +4785,7 @@
         <v>11</v>
       </c>
       <c r="D154" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E154" t="n" s="0">
         <v>2020.0</v>
@@ -4796,7 +4802,7 @@
         <v>198</v>
       </c>
       <c r="C155" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D155" t="s" s="0">
         <v>37</v>
@@ -4805,7 +4811,7 @@
         <v>2006.0</v>
       </c>
       <c r="F155" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="156">
@@ -4816,7 +4822,7 @@
         <v>199</v>
       </c>
       <c r="C156" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D156" t="s" s="0">
         <v>77</v>
@@ -4825,7 +4831,7 @@
         <v>2007.0</v>
       </c>
       <c r="F156" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="157">
@@ -4836,7 +4842,7 @@
         <v>200</v>
       </c>
       <c r="C157" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D157" t="s" s="0">
         <v>58</v>
@@ -4856,7 +4862,7 @@
         <v>201</v>
       </c>
       <c r="C158" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D158" t="s" s="0">
         <v>71</v>
@@ -4865,7 +4871,7 @@
         <v>2004.0</v>
       </c>
       <c r="F158" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="159">
@@ -4936,10 +4942,10 @@
         <v>205</v>
       </c>
       <c r="C162" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D162" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E162" t="n" s="0">
         <v>1985.0</v>
@@ -4956,7 +4962,7 @@
         <v>206</v>
       </c>
       <c r="C163" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D163" t="s" s="0">
         <v>88</v>
@@ -4976,16 +4982,16 @@
         <v>207</v>
       </c>
       <c r="C164" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D164" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E164" t="n" s="0">
         <v>1989.0</v>
       </c>
       <c r="F164" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="165">
@@ -4996,16 +5002,16 @@
         <v>208</v>
       </c>
       <c r="C165" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D165" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E165" t="n" s="0">
         <v>2005.0</v>
       </c>
       <c r="F165" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="166">
@@ -5016,10 +5022,10 @@
         <v>209</v>
       </c>
       <c r="C166" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D166" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E166" t="n" s="0">
         <v>2010.0</v>
@@ -5096,7 +5102,7 @@
         <v>213</v>
       </c>
       <c r="C170" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D170" t="s" s="0">
         <v>37</v>
@@ -5116,10 +5122,10 @@
         <v>214</v>
       </c>
       <c r="C171" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D171" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E171" t="n" s="0">
         <v>1992.0</v>
@@ -5156,7 +5162,7 @@
         <v>216</v>
       </c>
       <c r="C173" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D173" t="s" s="0">
         <v>217</v>
@@ -5165,7 +5171,7 @@
         <v>2015.0</v>
       </c>
       <c r="F173" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="174">
@@ -5196,7 +5202,7 @@
         <v>219</v>
       </c>
       <c r="C175" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D175" t="s" s="0">
         <v>39</v>
@@ -5205,7 +5211,7 @@
         <v>1988.0</v>
       </c>
       <c r="F175" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="176">
@@ -5245,7 +5251,7 @@
         <v>1989.0</v>
       </c>
       <c r="F177" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="178">
@@ -5256,10 +5262,10 @@
         <v>222</v>
       </c>
       <c r="C178" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D178" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E178" t="n" s="0">
         <v>2013.0</v>
@@ -5285,7 +5291,7 @@
         <v>2019.0</v>
       </c>
       <c r="F179" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="180">
@@ -5325,7 +5331,7 @@
         <v>1992.0</v>
       </c>
       <c r="F181" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="182">
@@ -5345,7 +5351,7 @@
         <v>1990.0</v>
       </c>
       <c r="F182" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="183">
@@ -5356,7 +5362,7 @@
         <v>227</v>
       </c>
       <c r="C183" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D183" t="s" s="0">
         <v>129</v>
@@ -5365,7 +5371,7 @@
         <v>1985.0</v>
       </c>
       <c r="F183" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="184">
@@ -5376,16 +5382,16 @@
         <v>228</v>
       </c>
       <c r="C184" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D184" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E184" t="n" s="0">
         <v>2005.0</v>
       </c>
       <c r="F184" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="185">
@@ -5425,7 +5431,7 @@
         <v>1992.0</v>
       </c>
       <c r="F186" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="187">
@@ -5445,7 +5451,7 @@
         <v>1998.0</v>
       </c>
       <c r="F187" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="188">
@@ -5456,10 +5462,10 @@
         <v>232</v>
       </c>
       <c r="C188" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D188" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E188" t="n" s="0">
         <v>2020.0</v>
@@ -5476,7 +5482,7 @@
         <v>233</v>
       </c>
       <c r="C189" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D189" t="s" s="0">
         <v>217</v>
@@ -5485,7 +5491,7 @@
         <v>1994.0</v>
       </c>
       <c r="F189" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="190">
@@ -5516,7 +5522,7 @@
         <v>235</v>
       </c>
       <c r="C191" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D191" t="s" s="0">
         <v>217</v>
@@ -5536,16 +5542,16 @@
         <v>236</v>
       </c>
       <c r="C192" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D192" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E192" t="n" s="0">
         <v>1999.0</v>
       </c>
       <c r="F192" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="193">
@@ -5556,7 +5562,7 @@
         <v>237</v>
       </c>
       <c r="C193" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D193" t="s" s="0">
         <v>129</v>
@@ -5565,7 +5571,7 @@
         <v>2001.0</v>
       </c>
       <c r="F193" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="194">
@@ -5605,7 +5611,7 @@
         <v>1995.0</v>
       </c>
       <c r="F195" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="196">
@@ -5616,7 +5622,7 @@
         <v>240</v>
       </c>
       <c r="C196" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D196" t="s" s="0">
         <v>88</v>
@@ -5625,7 +5631,7 @@
         <v>1991.0</v>
       </c>
       <c r="F196" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="197">
@@ -5665,7 +5671,7 @@
         <v>2018.0</v>
       </c>
       <c r="F198" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="199">
@@ -5685,7 +5691,7 @@
         <v>1991.0</v>
       </c>
       <c r="F199" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="200">
@@ -5705,7 +5711,7 @@
         <v>2010.0</v>
       </c>
       <c r="F200" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="201">
@@ -5716,10 +5722,10 @@
         <v>245</v>
       </c>
       <c r="C201" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D201" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E201" t="n" s="0">
         <v>2006.0</v>
@@ -5745,7 +5751,7 @@
         <v>2013.0</v>
       </c>
       <c r="F202" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="203">
@@ -5756,16 +5762,16 @@
         <v>247</v>
       </c>
       <c r="C203" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D203" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E203" t="n" s="0">
         <v>1996.0</v>
       </c>
       <c r="F203" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="204">
@@ -5776,10 +5782,10 @@
         <v>248</v>
       </c>
       <c r="C204" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D204" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E204" t="n" s="0">
         <v>2013.0</v>
@@ -5796,16 +5802,16 @@
         <v>249</v>
       </c>
       <c r="C205" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D205" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E205" t="n" s="0">
         <v>2012.0</v>
       </c>
       <c r="F205" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="206">
@@ -5816,16 +5822,16 @@
         <v>250</v>
       </c>
       <c r="C206" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D206" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E206" t="n" s="0">
         <v>1995.0</v>
       </c>
       <c r="F206" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="207">
@@ -5836,10 +5842,10 @@
         <v>251</v>
       </c>
       <c r="C207" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D207" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E207" t="n" s="0">
         <v>2022.0</v>
@@ -5856,16 +5862,16 @@
         <v>252</v>
       </c>
       <c r="C208" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D208" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E208" t="n" s="0">
         <v>2012.0</v>
       </c>
       <c r="F208" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="209">
@@ -5899,13 +5905,13 @@
         <v>11</v>
       </c>
       <c r="D210" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E210" t="n" s="0">
         <v>1986.0</v>
       </c>
       <c r="F210" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="211">
@@ -5916,10 +5922,10 @@
         <v>255</v>
       </c>
       <c r="C211" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D211" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E211" t="n" s="0">
         <v>2023.0</v>
@@ -5956,7 +5962,7 @@
         <v>257</v>
       </c>
       <c r="C213" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D213" t="s" s="0">
         <v>107</v>
@@ -5996,7 +6002,7 @@
         <v>259</v>
       </c>
       <c r="C215" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D215" t="s" s="0">
         <v>217</v>
@@ -6045,7 +6051,7 @@
         <v>2025.0</v>
       </c>
       <c r="F217" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="218">
@@ -6096,7 +6102,7 @@
         <v>264</v>
       </c>
       <c r="C220" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D220" t="s" s="0">
         <v>58</v>
@@ -6105,7 +6111,7 @@
         <v>2014.0</v>
       </c>
       <c r="F220" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="221">
@@ -6116,7 +6122,7 @@
         <v>265</v>
       </c>
       <c r="C221" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D221" t="s" s="0">
         <v>77</v>
@@ -6136,7 +6142,7 @@
         <v>266</v>
       </c>
       <c r="C222" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D222" t="s" s="0">
         <v>107</v>
@@ -6145,7 +6151,7 @@
         <v>1993.0</v>
       </c>
       <c r="F222" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="223">
@@ -6156,16 +6162,16 @@
         <v>267</v>
       </c>
       <c r="C223" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D223" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E223" t="n" s="0">
         <v>1992.0</v>
       </c>
       <c r="F223" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="224">
@@ -6216,7 +6222,7 @@
         <v>270</v>
       </c>
       <c r="C226" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D226" t="s" s="0">
         <v>39</v>
@@ -6236,10 +6242,10 @@
         <v>271</v>
       </c>
       <c r="C227" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D227" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E227" t="n" s="0">
         <v>1993.0</v>
@@ -6265,7 +6271,7 @@
         <v>1996.0</v>
       </c>
       <c r="F228" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="229">
@@ -6276,7 +6282,7 @@
         <v>273</v>
       </c>
       <c r="C229" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D229" t="s" s="0">
         <v>217</v>
@@ -6285,7 +6291,7 @@
         <v>1988.0</v>
       </c>
       <c r="F229" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="230">
@@ -6296,10 +6302,10 @@
         <v>274</v>
       </c>
       <c r="C230" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D230" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E230" t="n" s="0">
         <v>1985.0</v>
@@ -6316,10 +6322,10 @@
         <v>275</v>
       </c>
       <c r="C231" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D231" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E231" t="n" s="0">
         <v>2010.0</v>
@@ -6336,7 +6342,7 @@
         <v>276</v>
       </c>
       <c r="C232" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D232" t="s" s="0">
         <v>71</v>
@@ -6345,7 +6351,7 @@
         <v>2009.0</v>
       </c>
       <c r="F232" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="233">
@@ -6396,7 +6402,7 @@
         <v>279</v>
       </c>
       <c r="C235" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D235" t="s" s="0">
         <v>39</v>
@@ -6405,7 +6411,7 @@
         <v>2026.0</v>
       </c>
       <c r="F235" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="236">
@@ -6416,16 +6422,16 @@
         <v>280</v>
       </c>
       <c r="C236" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D236" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E236" t="n" s="0">
         <v>1994.0</v>
       </c>
       <c r="F236" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="237">
@@ -6436,10 +6442,10 @@
         <v>281</v>
       </c>
       <c r="C237" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D237" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E237" t="n" s="0">
         <v>1996.0</v>
@@ -6476,7 +6482,7 @@
         <v>283</v>
       </c>
       <c r="C239" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D239" t="s" s="0">
         <v>39</v>
@@ -6485,7 +6491,7 @@
         <v>1995.0</v>
       </c>
       <c r="F239" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="240">
@@ -6496,16 +6502,16 @@
         <v>284</v>
       </c>
       <c r="C240" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D240" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E240" t="n" s="0">
         <v>1991.0</v>
       </c>
       <c r="F240" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="241">
@@ -6525,7 +6531,7 @@
         <v>2014.0</v>
       </c>
       <c r="F241" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="242">
@@ -6536,16 +6542,16 @@
         <v>286</v>
       </c>
       <c r="C242" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D242" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E242" t="n" s="0">
         <v>2012.0</v>
       </c>
       <c r="F242" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="243">
@@ -6565,7 +6571,7 @@
         <v>1995.0</v>
       </c>
       <c r="F243" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="244">
@@ -6576,7 +6582,7 @@
         <v>288</v>
       </c>
       <c r="C244" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D244" t="s" s="0">
         <v>107</v>
@@ -6616,7 +6622,7 @@
         <v>290</v>
       </c>
       <c r="C246" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D246" t="s" s="0">
         <v>129</v>
@@ -6625,7 +6631,7 @@
         <v>1993.0</v>
       </c>
       <c r="F246" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="247">
@@ -6656,7 +6662,7 @@
         <v>292</v>
       </c>
       <c r="C248" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D248" t="s" s="0">
         <v>71</v>
@@ -6679,7 +6685,7 @@
         <v>11</v>
       </c>
       <c r="D249" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E249" t="n" s="0">
         <v>2021.0</v>
@@ -6756,16 +6762,16 @@
         <v>297</v>
       </c>
       <c r="C253" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D253" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E253" t="n" s="0">
         <v>2018.0</v>
       </c>
       <c r="F253" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="254">
@@ -6776,7 +6782,7 @@
         <v>298</v>
       </c>
       <c r="C254" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D254" t="s" s="0">
         <v>37</v>
@@ -6785,7 +6791,7 @@
         <v>2003.0</v>
       </c>
       <c r="F254" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="255">
@@ -6796,7 +6802,7 @@
         <v>299</v>
       </c>
       <c r="C255" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D255" t="s" s="0">
         <v>77</v>
@@ -6805,7 +6811,7 @@
         <v>2010.0</v>
       </c>
       <c r="F255" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="256">
@@ -6816,7 +6822,7 @@
         <v>300</v>
       </c>
       <c r="C256" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D256" t="s" s="0">
         <v>39</v>
@@ -6825,7 +6831,7 @@
         <v>2014.0</v>
       </c>
       <c r="F256" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="257">
@@ -6836,10 +6842,10 @@
         <v>301</v>
       </c>
       <c r="C257" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D257" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E257" t="n" s="0">
         <v>1997.0</v>
@@ -6856,7 +6862,7 @@
         <v>302</v>
       </c>
       <c r="C258" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D258" t="s" s="0">
         <v>107</v>
@@ -6865,7 +6871,7 @@
         <v>2002.0</v>
       </c>
       <c r="F258" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="259">
@@ -6876,7 +6882,7 @@
         <v>303</v>
       </c>
       <c r="C259" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D259" t="s" s="0">
         <v>39</v>
@@ -6896,7 +6902,7 @@
         <v>304</v>
       </c>
       <c r="C260" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D260" t="s" s="0">
         <v>39</v>
@@ -6965,7 +6971,7 @@
         <v>2017.0</v>
       </c>
       <c r="F263" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="264">
@@ -6985,7 +6991,7 @@
         <v>2016.0</v>
       </c>
       <c r="F264" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="265">
@@ -6996,7 +7002,7 @@
         <v>309</v>
       </c>
       <c r="C265" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D265" t="s" s="0">
         <v>37</v>
@@ -7005,7 +7011,7 @@
         <v>1986.0</v>
       </c>
       <c r="F265" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="266">
@@ -7036,7 +7042,7 @@
         <v>311</v>
       </c>
       <c r="C267" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D267" t="s" s="0">
         <v>39</v>
@@ -7045,7 +7051,7 @@
         <v>2020.0</v>
       </c>
       <c r="F267" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="268">
@@ -7056,7 +7062,7 @@
         <v>312</v>
       </c>
       <c r="C268" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D268" t="s" s="0">
         <v>71</v>
@@ -7096,7 +7102,7 @@
         <v>314</v>
       </c>
       <c r="C270" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D270" t="s" s="0">
         <v>71</v>
@@ -7125,7 +7131,7 @@
         <v>2015.0</v>
       </c>
       <c r="F271" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="272">
@@ -7136,7 +7142,7 @@
         <v>316</v>
       </c>
       <c r="C272" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D272" t="s" s="0">
         <v>217</v>
@@ -7145,7 +7151,7 @@
         <v>2024.0</v>
       </c>
       <c r="F272" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="273">
@@ -7176,7 +7182,7 @@
         <v>318</v>
       </c>
       <c r="C274" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D274" t="s" s="0">
         <v>37</v>
@@ -7196,7 +7202,7 @@
         <v>319</v>
       </c>
       <c r="C275" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D275" t="s" s="0">
         <v>39</v>
@@ -7205,7 +7211,7 @@
         <v>2016.0</v>
       </c>
       <c r="F275" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="276">
@@ -7216,10 +7222,10 @@
         <v>320</v>
       </c>
       <c r="C276" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D276" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E276" t="n" s="0">
         <v>2005.0</v>
@@ -7259,7 +7265,7 @@
         <v>11</v>
       </c>
       <c r="D278" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E278" t="n" s="0">
         <v>2024.0</v>
@@ -7276,10 +7282,10 @@
         <v>323</v>
       </c>
       <c r="C279" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D279" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E279" t="n" s="0">
         <v>2008.0</v>
@@ -7296,10 +7302,10 @@
         <v>324</v>
       </c>
       <c r="C280" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D280" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E280" t="n" s="0">
         <v>1988.0</v>
@@ -7316,7 +7322,7 @@
         <v>325</v>
       </c>
       <c r="C281" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D281" t="s" s="0">
         <v>58</v>
@@ -7336,7 +7342,7 @@
         <v>326</v>
       </c>
       <c r="C282" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D282" t="s" s="0">
         <v>71</v>
@@ -7345,7 +7351,7 @@
         <v>2024.0</v>
       </c>
       <c r="F282" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="283">
@@ -7365,7 +7371,7 @@
         <v>2004.0</v>
       </c>
       <c r="F283" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="284">
@@ -7376,7 +7382,7 @@
         <v>328</v>
       </c>
       <c r="C284" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D284" t="s" s="0">
         <v>88</v>
@@ -7385,7 +7391,7 @@
         <v>2014.0</v>
       </c>
       <c r="F284" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="285">
@@ -7425,7 +7431,7 @@
         <v>2001.0</v>
       </c>
       <c r="F286" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="287">
@@ -7436,7 +7442,7 @@
         <v>331</v>
       </c>
       <c r="C287" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D287" t="s" s="0">
         <v>58</v>
@@ -7445,7 +7451,7 @@
         <v>2007.0</v>
       </c>
       <c r="F287" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="288">
@@ -7465,7 +7471,7 @@
         <v>1996.0</v>
       </c>
       <c r="F288" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="289">
@@ -7476,7 +7482,7 @@
         <v>333</v>
       </c>
       <c r="C289" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D289" t="s" s="0">
         <v>129</v>
@@ -7485,7 +7491,7 @@
         <v>2009.0</v>
       </c>
       <c r="F289" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="290">
@@ -7496,16 +7502,16 @@
         <v>334</v>
       </c>
       <c r="C290" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D290" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E290" t="n" s="0">
         <v>2018.0</v>
       </c>
       <c r="F290" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="291">
@@ -7516,16 +7522,16 @@
         <v>335</v>
       </c>
       <c r="C291" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D291" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E291" t="n" s="0">
         <v>1996.0</v>
       </c>
       <c r="F291" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="292">
@@ -7545,7 +7551,7 @@
         <v>1996.0</v>
       </c>
       <c r="F292" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="293">
@@ -7556,10 +7562,10 @@
         <v>337</v>
       </c>
       <c r="C293" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D293" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E293" t="n" s="0">
         <v>2003.0</v>
@@ -7585,7 +7591,7 @@
         <v>2000.0</v>
       </c>
       <c r="F294" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="295">
@@ -7599,7 +7605,7 @@
         <v>11</v>
       </c>
       <c r="D295" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E295" t="n" s="0">
         <v>1990.0</v>
@@ -7616,10 +7622,10 @@
         <v>340</v>
       </c>
       <c r="C296" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D296" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E296" t="n" s="0">
         <v>2025.0</v>
@@ -7645,7 +7651,7 @@
         <v>1985.0</v>
       </c>
       <c r="F297" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="298">
@@ -7665,7 +7671,7 @@
         <v>2002.0</v>
       </c>
       <c r="F298" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="299">
@@ -7696,16 +7702,16 @@
         <v>344</v>
       </c>
       <c r="C300" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D300" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E300" t="n" s="0">
         <v>2018.0</v>
       </c>
       <c r="F300" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="301">
@@ -7725,7 +7731,7 @@
         <v>2026.0</v>
       </c>
       <c r="F301" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="302">
@@ -7799,13 +7805,13 @@
         <v>11</v>
       </c>
       <c r="D305" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E305" t="n" s="0">
         <v>1992.0</v>
       </c>
       <c r="F305" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="306">
@@ -7825,7 +7831,7 @@
         <v>1999.0</v>
       </c>
       <c r="F306" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="307">
@@ -7856,16 +7862,16 @@
         <v>352</v>
       </c>
       <c r="C308" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D308" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E308" t="n" s="0">
         <v>2021.0</v>
       </c>
       <c r="F308" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="309">
@@ -7876,7 +7882,7 @@
         <v>353</v>
       </c>
       <c r="C309" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D309" t="s" s="0">
         <v>217</v>
@@ -7899,13 +7905,13 @@
         <v>11</v>
       </c>
       <c r="D310" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E310" t="n" s="0">
         <v>1991.0</v>
       </c>
       <c r="F310" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="311">
@@ -7916,10 +7922,10 @@
         <v>355</v>
       </c>
       <c r="C311" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D311" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E311" t="n" s="0">
         <v>1989.0</v>
@@ -7976,7 +7982,7 @@
         <v>358</v>
       </c>
       <c r="C314" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D314" t="s" s="0">
         <v>107</v>
@@ -7985,7 +7991,7 @@
         <v>2010.0</v>
       </c>
       <c r="F314" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="315">
@@ -7996,16 +8002,16 @@
         <v>359</v>
       </c>
       <c r="C315" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D315" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E315" t="n" s="0">
         <v>1999.0</v>
       </c>
       <c r="F315" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="316">
@@ -8016,7 +8022,7 @@
         <v>360</v>
       </c>
       <c r="C316" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D316" t="s" s="0">
         <v>107</v>
@@ -8036,7 +8042,7 @@
         <v>361</v>
       </c>
       <c r="C317" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D317" t="s" s="0">
         <v>77</v>
@@ -8056,16 +8062,16 @@
         <v>362</v>
       </c>
       <c r="C318" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D318" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E318" t="n" s="0">
         <v>1985.0</v>
       </c>
       <c r="F318" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="319">
@@ -8076,7 +8082,7 @@
         <v>363</v>
       </c>
       <c r="C319" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D319" t="s" s="0">
         <v>71</v>
@@ -8116,7 +8122,7 @@
         <v>365</v>
       </c>
       <c r="C321" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D321" t="s" s="0">
         <v>107</v>
@@ -8125,7 +8131,7 @@
         <v>1985.0</v>
       </c>
       <c r="F321" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="322">
@@ -8176,7 +8182,7 @@
         <v>368</v>
       </c>
       <c r="C324" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D324" t="s" s="0">
         <v>88</v>
@@ -8196,10 +8202,10 @@
         <v>369</v>
       </c>
       <c r="C325" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D325" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E325" t="n" s="0">
         <v>2020.0</v>
@@ -8216,10 +8222,10 @@
         <v>370</v>
       </c>
       <c r="C326" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D326" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E326" t="n" s="0">
         <v>2012.0</v>
@@ -8236,10 +8242,10 @@
         <v>371</v>
       </c>
       <c r="C327" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D327" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E327" t="n" s="0">
         <v>2026.0</v>
@@ -8256,7 +8262,7 @@
         <v>372</v>
       </c>
       <c r="C328" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D328" t="s" s="0">
         <v>39</v>
@@ -8296,7 +8302,7 @@
         <v>374</v>
       </c>
       <c r="C330" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D330" t="s" s="0">
         <v>217</v>
@@ -8316,7 +8322,7 @@
         <v>375</v>
       </c>
       <c r="C331" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D331" t="s" s="0">
         <v>129</v>
@@ -8336,10 +8342,10 @@
         <v>376</v>
       </c>
       <c r="C332" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D332" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E332" t="n" s="0">
         <v>1996.0</v>
@@ -8365,7 +8371,7 @@
         <v>1995.0</v>
       </c>
       <c r="F333" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="334">
@@ -8376,7 +8382,7 @@
         <v>378</v>
       </c>
       <c r="C334" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D334" t="s" s="0">
         <v>58</v>
@@ -8396,16 +8402,16 @@
         <v>379</v>
       </c>
       <c r="C335" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D335" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E335" t="n" s="0">
         <v>2018.0</v>
       </c>
       <c r="F335" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="336">
@@ -8425,7 +8431,7 @@
         <v>2001.0</v>
       </c>
       <c r="F336" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="337">
@@ -8465,7 +8471,7 @@
         <v>2009.0</v>
       </c>
       <c r="F338" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="339">
@@ -8476,16 +8482,16 @@
         <v>383</v>
       </c>
       <c r="C339" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D339" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E339" t="n" s="0">
         <v>1992.0</v>
       </c>
       <c r="F339" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="340">
@@ -8545,7 +8551,7 @@
         <v>2006.0</v>
       </c>
       <c r="F342" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="343">
@@ -8565,7 +8571,7 @@
         <v>2003.0</v>
       </c>
       <c r="F343" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="344">
@@ -8605,7 +8611,7 @@
         <v>2011.0</v>
       </c>
       <c r="F345" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="346">
@@ -8625,7 +8631,7 @@
         <v>2013.0</v>
       </c>
       <c r="F346" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="347">
@@ -8636,10 +8642,10 @@
         <v>391</v>
       </c>
       <c r="C347" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D347" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E347" t="n" s="0">
         <v>1997.0</v>
@@ -8656,7 +8662,7 @@
         <v>392</v>
       </c>
       <c r="C348" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D348" t="s" s="0">
         <v>129</v>
@@ -8665,7 +8671,7 @@
         <v>2022.0</v>
       </c>
       <c r="F348" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="349">
@@ -8676,16 +8682,16 @@
         <v>393</v>
       </c>
       <c r="C349" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D349" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E349" t="n" s="0">
         <v>1991.0</v>
       </c>
       <c r="F349" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="350">
@@ -8696,7 +8702,7 @@
         <v>394</v>
       </c>
       <c r="C350" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D350" t="s" s="0">
         <v>217</v>
@@ -8705,7 +8711,7 @@
         <v>2002.0</v>
       </c>
       <c r="F350" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="351">
@@ -8725,7 +8731,7 @@
         <v>1986.0</v>
       </c>
       <c r="F351" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="352">
@@ -8736,10 +8742,10 @@
         <v>396</v>
       </c>
       <c r="C352" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D352" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E352" t="n" s="0">
         <v>2018.0</v>
@@ -8756,10 +8762,10 @@
         <v>397</v>
       </c>
       <c r="C353" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D353" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E353" t="n" s="0">
         <v>2011.0</v>
@@ -8776,7 +8782,7 @@
         <v>398</v>
       </c>
       <c r="C354" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D354" t="s" s="0">
         <v>217</v>
@@ -8785,7 +8791,7 @@
         <v>2014.0</v>
       </c>
       <c r="F354" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="355">
@@ -8796,7 +8802,7 @@
         <v>399</v>
       </c>
       <c r="C355" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D355" t="s" s="0">
         <v>217</v>
@@ -8816,10 +8822,10 @@
         <v>400</v>
       </c>
       <c r="C356" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D356" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E356" t="n" s="0">
         <v>1985.0</v>
@@ -8836,7 +8842,7 @@
         <v>401</v>
       </c>
       <c r="C357" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D357" t="s" s="0">
         <v>37</v>
@@ -8845,7 +8851,7 @@
         <v>2024.0</v>
       </c>
       <c r="F357" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="358">
@@ -8885,7 +8891,7 @@
         <v>1997.0</v>
       </c>
       <c r="F359" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="360">
@@ -8896,7 +8902,7 @@
         <v>404</v>
       </c>
       <c r="C360" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D360" t="s" s="0">
         <v>217</v>
@@ -8945,7 +8951,7 @@
         <v>2013.0</v>
       </c>
       <c r="F362" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="363">
@@ -9005,7 +9011,7 @@
         <v>2013.0</v>
       </c>
       <c r="F365" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="366">
@@ -9039,7 +9045,7 @@
         <v>11</v>
       </c>
       <c r="D367" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E367" t="n" s="0">
         <v>1992.0</v>
@@ -9065,7 +9071,7 @@
         <v>2008.0</v>
       </c>
       <c r="F368" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="369">
@@ -9076,7 +9082,7 @@
         <v>413</v>
       </c>
       <c r="C369" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D369" t="s" s="0">
         <v>71</v>
@@ -9116,7 +9122,7 @@
         <v>415</v>
       </c>
       <c r="C371" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D371" t="s" s="0">
         <v>37</v>
@@ -9136,7 +9142,7 @@
         <v>416</v>
       </c>
       <c r="C372" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D372" t="s" s="0">
         <v>107</v>
@@ -9156,7 +9162,7 @@
         <v>417</v>
       </c>
       <c r="C373" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D373" t="s" s="0">
         <v>107</v>
@@ -9185,7 +9191,7 @@
         <v>2003.0</v>
       </c>
       <c r="F374" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="375">
@@ -9279,13 +9285,13 @@
         <v>11</v>
       </c>
       <c r="D379" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E379" t="n" s="0">
         <v>2006.0</v>
       </c>
       <c r="F379" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="380">
@@ -9316,10 +9322,10 @@
         <v>425</v>
       </c>
       <c r="C381" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D381" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E381" t="n" s="0">
         <v>2010.0</v>
@@ -9365,7 +9371,7 @@
         <v>2020.0</v>
       </c>
       <c r="F383" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="384">
@@ -9376,10 +9382,10 @@
         <v>428</v>
       </c>
       <c r="C384" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D384" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E384" t="n" s="0">
         <v>1999.0</v>
@@ -9405,7 +9411,7 @@
         <v>2014.0</v>
       </c>
       <c r="F385" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="386">
@@ -9416,7 +9422,7 @@
         <v>430</v>
       </c>
       <c r="C386" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D386" t="s" s="0">
         <v>37</v>
@@ -9465,7 +9471,7 @@
         <v>2003.0</v>
       </c>
       <c r="F388" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="389">
@@ -9476,7 +9482,7 @@
         <v>433</v>
       </c>
       <c r="C389" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D389" t="s" s="0">
         <v>107</v>
@@ -9565,7 +9571,7 @@
         <v>2026.0</v>
       </c>
       <c r="F393" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="394">
@@ -9596,10 +9602,10 @@
         <v>439</v>
       </c>
       <c r="C395" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D395" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E395" t="n" s="0">
         <v>2008.0</v>
@@ -9616,7 +9622,7 @@
         <v>440</v>
       </c>
       <c r="C396" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D396" t="s" s="0">
         <v>129</v>
@@ -9625,7 +9631,7 @@
         <v>1999.0</v>
       </c>
       <c r="F396" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="397">
@@ -9685,7 +9691,7 @@
         <v>1996.0</v>
       </c>
       <c r="F399" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="400">
@@ -9696,7 +9702,7 @@
         <v>444</v>
       </c>
       <c r="C400" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D400" t="s" s="0">
         <v>107</v>
@@ -9776,7 +9782,7 @@
         <v>448</v>
       </c>
       <c r="C404" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D404" t="s" s="0">
         <v>88</v>
@@ -9825,7 +9831,7 @@
         <v>1997.0</v>
       </c>
       <c r="F406" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="407">
@@ -9856,10 +9862,10 @@
         <v>452</v>
       </c>
       <c r="C408" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D408" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E408" t="n" s="0">
         <v>1998.0</v>
@@ -9876,7 +9882,7 @@
         <v>453</v>
       </c>
       <c r="C409" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D409" t="s" s="0">
         <v>217</v>
@@ -9916,10 +9922,10 @@
         <v>455</v>
       </c>
       <c r="C411" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D411" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E411" t="n" s="0">
         <v>2006.0</v>
@@ -9945,7 +9951,7 @@
         <v>2023.0</v>
       </c>
       <c r="F412" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="413">
@@ -9965,7 +9971,7 @@
         <v>1999.0</v>
       </c>
       <c r="F413" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="414">
@@ -9976,7 +9982,7 @@
         <v>458</v>
       </c>
       <c r="C414" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D414" t="s" s="0">
         <v>107</v>
@@ -9996,7 +10002,7 @@
         <v>459</v>
       </c>
       <c r="C415" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D415" t="s" s="0">
         <v>39</v>
@@ -10005,7 +10011,7 @@
         <v>2014.0</v>
       </c>
       <c r="F415" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="416">
@@ -10016,7 +10022,7 @@
         <v>460</v>
       </c>
       <c r="C416" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D416" t="s" s="0">
         <v>58</v>
@@ -10025,7 +10031,7 @@
         <v>2002.0</v>
       </c>
       <c r="F416" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="417">
@@ -10036,10 +10042,10 @@
         <v>461</v>
       </c>
       <c r="C417" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D417" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E417" t="n" s="0">
         <v>1995.0</v>
@@ -10056,10 +10062,10 @@
         <v>462</v>
       </c>
       <c r="C418" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D418" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E418" t="n" s="0">
         <v>2002.0</v>
@@ -10076,10 +10082,10 @@
         <v>463</v>
       </c>
       <c r="C419" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D419" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E419" t="n" s="0">
         <v>1985.0</v>
@@ -10105,7 +10111,7 @@
         <v>2002.0</v>
       </c>
       <c r="F420" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="421">
@@ -10165,7 +10171,7 @@
         <v>2010.0</v>
       </c>
       <c r="F423" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="424">
@@ -10176,7 +10182,7 @@
         <v>468</v>
       </c>
       <c r="C424" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D424" t="s" s="0">
         <v>107</v>
@@ -10205,7 +10211,7 @@
         <v>2022.0</v>
       </c>
       <c r="F425" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="426">
@@ -10245,7 +10251,7 @@
         <v>1986.0</v>
       </c>
       <c r="F427" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="428">
@@ -10256,7 +10262,7 @@
         <v>472</v>
       </c>
       <c r="C428" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D428" t="s" s="0">
         <v>217</v>
@@ -10276,7 +10282,7 @@
         <v>473</v>
       </c>
       <c r="C429" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D429" t="s" s="0">
         <v>71</v>
@@ -10285,7 +10291,7 @@
         <v>2011.0</v>
       </c>
       <c r="F429" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="430">
@@ -10296,7 +10302,7 @@
         <v>474</v>
       </c>
       <c r="C430" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D430" t="s" s="0">
         <v>107</v>
@@ -10316,7 +10322,7 @@
         <v>475</v>
       </c>
       <c r="C431" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D431" t="s" s="0">
         <v>77</v>
@@ -10336,7 +10342,7 @@
         <v>476</v>
       </c>
       <c r="C432" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D432" t="s" s="0">
         <v>77</v>
@@ -10345,7 +10351,7 @@
         <v>2016.0</v>
       </c>
       <c r="F432" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="433">
@@ -10356,7 +10362,7 @@
         <v>477</v>
       </c>
       <c r="C433" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D433" t="s" s="0">
         <v>217</v>
@@ -10405,7 +10411,7 @@
         <v>2018.0</v>
       </c>
       <c r="F435" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="436">
@@ -10445,7 +10451,7 @@
         <v>2001.0</v>
       </c>
       <c r="F437" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="438">
@@ -10465,7 +10471,7 @@
         <v>1988.0</v>
       </c>
       <c r="F438" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="439">
@@ -10476,10 +10482,10 @@
         <v>483</v>
       </c>
       <c r="C439" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D439" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E439" t="n" s="0">
         <v>1993.0</v>
@@ -10505,7 +10511,7 @@
         <v>2009.0</v>
       </c>
       <c r="F440" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="441">
@@ -10525,7 +10531,7 @@
         <v>2019.0</v>
       </c>
       <c r="F441" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="442">
@@ -10585,7 +10591,7 @@
         <v>1986.0</v>
       </c>
       <c r="F444" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="445">
@@ -10596,7 +10602,7 @@
         <v>489</v>
       </c>
       <c r="C445" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D445" t="s" s="0">
         <v>71</v>
@@ -10605,7 +10611,7 @@
         <v>2017.0</v>
       </c>
       <c r="F445" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="446">
@@ -10625,7 +10631,7 @@
         <v>2026.0</v>
       </c>
       <c r="F446" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="447">
@@ -10665,7 +10671,7 @@
         <v>2019.0</v>
       </c>
       <c r="F448" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="449">
@@ -10676,7 +10682,7 @@
         <v>493</v>
       </c>
       <c r="C449" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D449" t="s" s="0">
         <v>39</v>
@@ -10736,7 +10742,7 @@
         <v>496</v>
       </c>
       <c r="C452" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D452" t="s" s="0">
         <v>107</v>
@@ -10745,7 +10751,7 @@
         <v>1995.0</v>
       </c>
       <c r="F452" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="453">
@@ -10776,7 +10782,7 @@
         <v>498</v>
       </c>
       <c r="C454" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D454" t="s" s="0">
         <v>217</v>
@@ -10799,7 +10805,7 @@
         <v>11</v>
       </c>
       <c r="D455" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E455" t="n" s="0">
         <v>2011.0</v>
@@ -10819,13 +10825,13 @@
         <v>11</v>
       </c>
       <c r="D456" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E456" t="n" s="0">
         <v>2013.0</v>
       </c>
       <c r="F456" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="457">
@@ -10836,7 +10842,7 @@
         <v>501</v>
       </c>
       <c r="C457" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D457" t="s" s="0">
         <v>88</v>
@@ -10845,7 +10851,7 @@
         <v>2003.0</v>
       </c>
       <c r="F457" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="458">
@@ -10859,7 +10865,7 @@
         <v>11</v>
       </c>
       <c r="D458" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E458" t="n" s="0">
         <v>2005.0</v>
@@ -10876,7 +10882,7 @@
         <v>503</v>
       </c>
       <c r="C459" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D459" t="s" s="0">
         <v>88</v>
@@ -10936,7 +10942,7 @@
         <v>506</v>
       </c>
       <c r="C462" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D462" t="s" s="0">
         <v>88</v>
@@ -10945,7 +10951,7 @@
         <v>1998.0</v>
       </c>
       <c r="F462" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="463">
@@ -10956,7 +10962,7 @@
         <v>507</v>
       </c>
       <c r="C463" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D463" t="s" s="0">
         <v>129</v>
@@ -10996,7 +11002,7 @@
         <v>509</v>
       </c>
       <c r="C465" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D465" t="s" s="0">
         <v>217</v>
@@ -11036,16 +11042,16 @@
         <v>511</v>
       </c>
       <c r="C467" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D467" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E467" t="n" s="0">
         <v>2001.0</v>
       </c>
       <c r="F467" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="468">
@@ -11085,7 +11091,7 @@
         <v>1987.0</v>
       </c>
       <c r="F469" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="470">
@@ -11096,10 +11102,10 @@
         <v>514</v>
       </c>
       <c r="C470" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D470" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E470" t="n" s="0">
         <v>2017.0</v>
@@ -11145,7 +11151,7 @@
         <v>2008.0</v>
       </c>
       <c r="F472" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="473">
@@ -11156,7 +11162,7 @@
         <v>517</v>
       </c>
       <c r="C473" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D473" t="s" s="0">
         <v>217</v>
@@ -11165,7 +11171,7 @@
         <v>2021.0</v>
       </c>
       <c r="F473" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="474">
@@ -11185,7 +11191,7 @@
         <v>2020.0</v>
       </c>
       <c r="F474" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="475">
@@ -11196,7 +11202,7 @@
         <v>519</v>
       </c>
       <c r="C475" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D475" t="s" s="0">
         <v>58</v>
@@ -11205,7 +11211,7 @@
         <v>2009.0</v>
       </c>
       <c r="F475" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="476">
@@ -11245,7 +11251,7 @@
         <v>1988.0</v>
       </c>
       <c r="F477" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="478">
@@ -11256,10 +11262,10 @@
         <v>522</v>
       </c>
       <c r="C478" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D478" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E478" t="n" s="0">
         <v>2001.0</v>
@@ -11296,10 +11302,10 @@
         <v>524</v>
       </c>
       <c r="C480" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D480" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E480" t="n" s="0">
         <v>2006.0</v>
@@ -11316,16 +11322,16 @@
         <v>525</v>
       </c>
       <c r="C481" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D481" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E481" t="n" s="0">
         <v>2009.0</v>
       </c>
       <c r="F481" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="482">
@@ -11336,10 +11342,10 @@
         <v>526</v>
       </c>
       <c r="C482" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D482" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E482" t="n" s="0">
         <v>2019.0</v>
@@ -11359,7 +11365,7 @@
         <v>11</v>
       </c>
       <c r="D483" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E483" t="n" s="0">
         <v>1997.0</v>
@@ -11376,7 +11382,7 @@
         <v>528</v>
       </c>
       <c r="C484" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D484" t="s" s="0">
         <v>71</v>
@@ -11405,7 +11411,7 @@
         <v>1990.0</v>
       </c>
       <c r="F485" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="486">
@@ -11439,7 +11445,7 @@
         <v>11</v>
       </c>
       <c r="D487" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E487" t="n" s="0">
         <v>1995.0</v>
@@ -11485,7 +11491,7 @@
         <v>2009.0</v>
       </c>
       <c r="F489" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="490">
@@ -11505,7 +11511,7 @@
         <v>2004.0</v>
       </c>
       <c r="F490" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="491">
@@ -11536,16 +11542,16 @@
         <v>536</v>
       </c>
       <c r="C492" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D492" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E492" t="n" s="0">
         <v>2020.0</v>
       </c>
       <c r="F492" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="493">
@@ -11579,7 +11585,7 @@
         <v>11</v>
       </c>
       <c r="D494" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E494" t="n" s="0">
         <v>2023.0</v>
@@ -11619,13 +11625,13 @@
         <v>11</v>
       </c>
       <c r="D496" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E496" t="n" s="0">
         <v>2011.0</v>
       </c>
       <c r="F496" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="497">
@@ -11636,7 +11642,7 @@
         <v>541</v>
       </c>
       <c r="C497" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D497" t="s" s="0">
         <v>71</v>
@@ -11645,7 +11651,7 @@
         <v>2005.0</v>
       </c>
       <c r="F497" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="498">
@@ -11665,7 +11671,7 @@
         <v>2011.0</v>
       </c>
       <c r="F498" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="499">
@@ -11676,10 +11682,10 @@
         <v>543</v>
       </c>
       <c r="C499" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D499" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E499" t="n" s="0">
         <v>1998.0</v>
@@ -11725,6 +11731,26 @@
         <v>2013.0</v>
       </c>
       <c r="F501" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="n" s="0">
+        <v>100500.0</v>
+      </c>
+      <c r="B502" t="s" s="0">
+        <v>546</v>
+      </c>
+      <c r="C502" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D502" t="s" s="0">
+        <v>547</v>
+      </c>
+      <c r="E502" t="n" s="0">
+        <v>2020.0</v>
+      </c>
+      <c r="F502" t="s" s="0">
         <v>9</v>
       </c>
     </row>

</xml_diff>